<commit_message>
Filter Translations for TaxonomyMeta
</commit_message>
<xml_diff>
--- a/database/imports/taxonomies.xlsx
+++ b/database/imports/taxonomies.xlsx
@@ -8,19 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Codes\PHP\Laravel\LaravelOcadmin\laraocadmin10\httpdocs\database\imports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B640F3C-84B3-45F4-8A8B-D8336F9E686C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B95D093-95DD-4A1B-8A8A-A650056AC8E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2115" yWindow="1095" windowWidth="21600" windowHeight="13680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="taxonomies" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="54">
   <si>
     <t>id</t>
   </si>
@@ -122,10 +135,92 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>2023/6/9  12:00</t>
-  </si>
-  <si>
-    <t>2023-10-21 21:20</t>
+    <t>CarBrand</t>
+  </si>
+  <si>
+    <t>App\Models\Catalog\Car</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>CarModel</t>
+  </si>
+  <si>
+    <t>廠牌</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>車型</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>車身樣式</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>排氣量</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>動力系統</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>CarBodyStyle</t>
+  </si>
+  <si>
+    <t>外觀顏色</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>內裝顏色</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>CarGeneration</t>
+  </si>
+  <si>
+    <t>世代</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>引擎類型</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>馬力</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023/6/912:00</t>
+  </si>
+  <si>
+    <t>2023-10-2121:20</t>
+  </si>
+  <si>
+    <t>2023-10-2218:00</t>
+  </si>
+  <si>
+    <t>CarEngineCapacity</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>CarPowertrain</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>CarEngineType</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>CarExteriorColor</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>CarInteriorColor</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>CarHorsepower</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1081,10 +1176,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <pane ySplit="2" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -1095,7 +1191,7 @@
     <col min="6" max="6" width="18.125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1115,7 +1211,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>24</v>
       </c>
@@ -1135,7 +1231,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1149,13 +1245,13 @@
         <v>1</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1169,13 +1265,13 @@
         <v>1</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1189,13 +1285,13 @@
         <v>1</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1209,13 +1305,13 @@
         <v>1</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1229,13 +1325,13 @@
         <v>1</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1249,13 +1345,13 @@
         <v>1</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1269,13 +1365,13 @@
         <v>1</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1289,13 +1385,13 @@
         <v>1</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -1309,13 +1405,13 @@
         <v>1</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -1329,13 +1425,13 @@
         <v>1</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
@@ -1349,13 +1445,13 @@
         <v>1</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
@@ -1369,13 +1465,13 @@
         <v>1</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
@@ -1389,10 +1485,240 @@
         <v>1</v>
       </c>
       <c r="E15" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" t="s">
         <v>31</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G16" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" t="s">
         <v>31</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G17" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" t="s">
+        <v>31</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G18" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" t="s">
+        <v>31</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G19" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
+        <v>48</v>
+      </c>
+      <c r="C20" t="s">
+        <v>31</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G20" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
+        <v>49</v>
+      </c>
+      <c r="C21" t="s">
+        <v>31</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G21" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
+        <v>50</v>
+      </c>
+      <c r="C22" t="s">
+        <v>31</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G22" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>21</v>
+      </c>
+      <c r="B23" t="s">
+        <v>51</v>
+      </c>
+      <c r="C23" t="s">
+        <v>31</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G23" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>22</v>
+      </c>
+      <c r="B24" t="s">
+        <v>52</v>
+      </c>
+      <c r="C24" t="s">
+        <v>31</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G24" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>23</v>
+      </c>
+      <c r="B25" t="s">
+        <v>53</v>
+      </c>
+      <c r="C25" t="s">
+        <v>31</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G25" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>